<commit_message>
made some progress plus more power points
</commit_message>
<xml_diff>
--- a/AI Testing.xlsx
+++ b/AI Testing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmcke\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmcke\Documents\gitStuff\FYP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{431ED41B-2596-4ABC-9461-9F2206727238}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92E8AAD-EA44-4258-B0A4-AE4729A1D266}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="7"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart8" sheetId="9" r:id="rId1"/>
@@ -138,7 +138,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1116,6 +1116,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Average Score at</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> Varied training</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1312,6 +1342,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Training</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Epochs</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1375,6 +1465,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Accuracy Score</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1476,6 +1621,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Average Score</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> at Varied Training</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1672,6 +1847,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Training Epochs</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1717,6 +1947,7 @@
         <c:axId val="144110064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="10"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1734,6 +1965,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Accuracy</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Score</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2031,6 +2322,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Training</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Epochs</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2094,6 +2445,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Accuracy Score</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB" sz="400">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2195,6 +2606,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Average Score at Varied Training</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1100">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2391,6 +2832,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Training</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Epochs</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2454,6 +2955,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Accuracy Score</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -20753,7 +21309,7 @@
 </file>
 
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="86" workbookViewId="0" zoomToFit="1"/>
@@ -20764,7 +21320,7 @@
 </file>
 
 <file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="86" workbookViewId="0" zoomToFit="1"/>
@@ -20775,7 +21331,7 @@
 </file>
 
 <file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="86" workbookViewId="0" zoomToFit="1"/>
@@ -20786,7 +21342,7 @@
 </file>
 
 <file path=xl/chartsheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="86" workbookViewId="0" zoomToFit="1"/>
@@ -20797,7 +21353,7 @@
 </file>
 
 <file path=xl/chartsheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="86" workbookViewId="0" zoomToFit="1"/>
@@ -20808,7 +21364,7 @@
 </file>
 
 <file path=xl/chartsheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="86" workbookViewId="0" zoomToFit="1"/>
@@ -20819,7 +21375,7 @@
 </file>
 
 <file path=xl/chartsheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="86" workbookViewId="0" zoomToFit="1"/>
@@ -21137,15 +21693,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>33337</xdr:colOff>
+      <xdr:colOff>233362</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>338137</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>538162</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -21685,11 +22241,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="C1:X141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D122" workbookViewId="0">
-      <selection activeCell="J144" sqref="J144"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="W89" sqref="W89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>